<commit_message>
Added dynamic values to TD
</commit_message>
<xml_diff>
--- a/public/file.xlsx
+++ b/public/file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="462" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="301" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -575,13 +575,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0%"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.00%"/>
     <numFmt numFmtId="168" formatCode="0.00"/>
-    <numFmt numFmtId="169" formatCode="0.00%"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -670,7 +669,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -691,14 +690,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -711,7 +702,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -795,7 +790,7 @@
   <dimension ref="A1:ED4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1249,350 +1244,350 @@
       <c r="S2" s="4" t="n">
         <v>0.0085542471378061</v>
       </c>
-      <c r="T2" s="4" t="n">
-        <v>0.0089680061019089</v>
-      </c>
-      <c r="U2" s="4" t="n">
-        <v>0.00932918878322026</v>
-      </c>
-      <c r="V2" s="4" t="n">
-        <v>0.0096459956148867</v>
-      </c>
-      <c r="W2" s="4" t="n">
-        <v>0.00992592896344995</v>
-      </c>
-      <c r="X2" s="4" t="n">
-        <v>0.0101729924814026</v>
-      </c>
-      <c r="Y2" s="4" t="n">
-        <v>0.0103938610007936</v>
-      </c>
-      <c r="Z2" s="4" t="n">
-        <v>0.010592811600659</v>
-      </c>
-      <c r="AA2" s="4" t="n">
-        <v>0.0107727388451816</v>
-      </c>
-      <c r="AB2" s="4" t="n">
-        <v>0.0109376717967745</v>
-      </c>
-      <c r="AC2" s="4" t="n">
-        <v>0.0110892342411869</v>
-      </c>
-      <c r="AD2" s="4" t="n">
-        <v>0.0112292836147036</v>
-      </c>
-      <c r="AE2" s="4" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="AF2" s="4" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="AG2" s="4" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="AH2" s="4" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="AI2" s="4" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="AJ2" s="4" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="AK2" s="4" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="AL2" s="4" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="AM2" s="4" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="AN2" s="4" t="n">
-        <v>0.280678788437129</v>
-      </c>
-      <c r="AO2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="4" t="n">
-        <v>0.186080348676564</v>
-      </c>
-      <c r="AQ2" s="4" t="n">
-        <v>0.198636414537903</v>
-      </c>
-      <c r="AR2" s="4" t="n">
-        <v>0.210570072303585</v>
-      </c>
-      <c r="AS2" s="4" t="n">
-        <v>0.221939427228588</v>
-      </c>
-      <c r="AT2" s="4" t="n">
-        <v>0.23279432512823</v>
-      </c>
-      <c r="AU2" s="4" t="n">
-        <v>0.243177804816212</v>
-      </c>
-      <c r="AV2" s="4" t="n">
-        <v>0.253127252250246</v>
-      </c>
-      <c r="AW2" s="4" t="n">
-        <v>0.262675329265581</v>
-      </c>
-      <c r="AX2" s="4" t="n">
-        <v>0.271850728031435</v>
-      </c>
-      <c r="AY2" s="4" t="n">
-        <v>0.280678788437129</v>
-      </c>
-      <c r="AZ2" s="4" t="n">
-        <v>0.289182006285979</v>
-      </c>
-      <c r="BA2" s="4" t="n">
-        <v>0.297380453666538</v>
-      </c>
-      <c r="BB2" s="4" t="n">
-        <v>0.305292128167705</v>
-      </c>
-      <c r="BC2" s="4" t="n">
-        <v>0.312933244106528</v>
-      </c>
-      <c r="BD2" s="4" t="n">
-        <v>0.32031847627676</v>
-      </c>
-      <c r="BE2" s="4" t="n">
-        <v>0.327461164666399</v>
-      </c>
-      <c r="BF2" s="4" t="n">
-        <v>0.334373486976474</v>
-      </c>
-      <c r="BG2" s="4" t="n">
-        <v>0.341066604492713</v>
-      </c>
-      <c r="BH2" s="4" t="n">
-        <v>0.347550785838943</v>
-      </c>
-      <c r="BI2" s="4" t="n">
-        <v>0.35383551231919</v>
-      </c>
-      <c r="BJ2" s="4" t="n">
-        <v>0.359929567891836</v>
-      </c>
-      <c r="BK2" s="5" t="n">
-        <v>1.95852876300086</v>
-      </c>
-      <c r="BL2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM2" s="5" t="n">
-        <v>1.55483903431484</v>
-      </c>
-      <c r="BN2" s="5" t="n">
-        <v>1.60221120254177</v>
-      </c>
-      <c r="BO2" s="5" t="n">
-        <v>1.64880974666206</v>
-      </c>
-      <c r="BP2" s="5" t="n">
-        <v>1.69470783641438</v>
-      </c>
-      <c r="BQ2" s="5" t="n">
-        <v>1.73996932818106</v>
-      </c>
-      <c r="BR2" s="5" t="n">
-        <v>1.78465088452399</v>
-      </c>
-      <c r="BS2" s="5" t="n">
-        <v>1.82880341532063</v>
-      </c>
-      <c r="BT2" s="5" t="n">
-        <v>1.87247307832556</v>
-      </c>
-      <c r="BU2" s="5" t="n">
-        <v>1.91570199250673</v>
-      </c>
-      <c r="BV2" s="5" t="n">
-        <v>1.95852876300086</v>
-      </c>
-      <c r="BW2" s="5" t="n">
-        <v>2.00098888141136</v>
-      </c>
-      <c r="BX2" s="5" t="n">
-        <v>2.0431150425505</v>
-      </c>
-      <c r="BY2" s="5" t="n">
-        <v>2.08493740415431</v>
-      </c>
-      <c r="BZ2" s="5" t="n">
-        <v>2.12648380671346</v>
-      </c>
-      <c r="CA2" s="5" t="n">
-        <v>2.16777996452198</v>
-      </c>
-      <c r="CB2" s="5" t="n">
-        <v>2.20884963516197</v>
-      </c>
-      <c r="CC2" s="5" t="n">
-        <v>2.2497147721528</v>
-      </c>
-      <c r="CD2" s="5" t="n">
-        <v>2.29039566390038</v>
-      </c>
-      <c r="CE2" s="5" t="n">
-        <v>2.33091106106971</v>
-      </c>
-      <c r="CF2" s="5" t="n">
-        <v>2.37127829386074</v>
-      </c>
-      <c r="CG2" s="5" t="n">
-        <v>2.41151338026375</v>
-      </c>
-      <c r="CH2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="CI2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="CJ2" s="6" t="n">
-        <v>0.0113597737310146</v>
+      <c r="T2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="X2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="AF2" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="AG2" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AH2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="AI2" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="AJ2" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="AK2" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AL2" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="AM2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="AN2" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AO2" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="AP2" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ2" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AR2" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AS2" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="AT2" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AU2" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AV2" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="AW2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AX2" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="AY2" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AZ2" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="BA2" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="BB2" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="BC2" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="BD2" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="BE2" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="BF2" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="BG2" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="BH2" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="BI2" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="BJ2" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="BK2" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="BL2" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="BM2" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="BN2" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="BO2" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="BP2" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="BQ2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="BR2" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="BS2" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="BT2" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="BU2" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="BV2" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="BW2" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="BX2" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="BY2" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="BZ2" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="CA2" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="CB2" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="CC2" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="CD2" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="CE2" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="CF2" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="CG2" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="CH2" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="CI2" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="CJ2" s="0" t="n">
+        <v>69</v>
       </c>
       <c r="CK2" s="0" t="n">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="CL2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM2" s="6" t="n">
-        <v>0.0085542471378061</v>
-      </c>
-      <c r="CN2" s="6" t="n">
-        <v>0.0089680061019089</v>
-      </c>
-      <c r="CO2" s="6" t="n">
-        <v>0.00932918878322026</v>
-      </c>
-      <c r="CP2" s="6" t="n">
-        <v>0.0096459956148867</v>
-      </c>
-      <c r="CQ2" s="6" t="n">
-        <v>0.00992592896344995</v>
-      </c>
-      <c r="CR2" s="6" t="n">
-        <v>0.0101729924814026</v>
-      </c>
-      <c r="CS2" s="6" t="n">
-        <v>0.0103938610007936</v>
-      </c>
-      <c r="CT2" s="6" t="n">
-        <v>0.010592811600659</v>
-      </c>
-      <c r="CU2" s="6" t="n">
-        <v>0.0107727388451816</v>
-      </c>
-      <c r="CV2" s="6" t="n">
-        <v>0.0109376717967745</v>
-      </c>
-      <c r="CW2" s="6" t="n">
-        <v>0.0110892342411869</v>
-      </c>
-      <c r="CX2" s="6" t="n">
-        <v>0.0112292836147036</v>
-      </c>
-      <c r="CY2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="CZ2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="DA2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="DB2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="DC2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="DD2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="DE2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="DF2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="DG2" s="6" t="n">
-        <v>0.0113597737310146</v>
+        <v>71</v>
+      </c>
+      <c r="CM2" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="CN2" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="CO2" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="CP2" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="CQ2" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="CR2" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="CS2" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="CT2" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="CU2" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="CV2" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="CW2" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="CX2" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="CY2" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="CZ2" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="DA2" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="DB2" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="DC2" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="DD2" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="DE2" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="DF2" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="DG2" s="0" t="n">
+        <v>92</v>
       </c>
       <c r="DH2" s="0" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="DI2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="DJ2" s="6" t="n">
-        <v>0.0085542471378061</v>
-      </c>
-      <c r="DK2" s="6" t="n">
-        <v>0.0089680061019089</v>
-      </c>
-      <c r="DL2" s="6" t="n">
-        <v>0.00932918878322026</v>
-      </c>
-      <c r="DM2" s="6" t="n">
-        <v>0.0096459956148867</v>
-      </c>
-      <c r="DN2" s="6" t="n">
-        <v>0.00992592896344995</v>
-      </c>
-      <c r="DO2" s="6" t="n">
-        <v>0.0101729924814026</v>
-      </c>
-      <c r="DP2" s="6" t="n">
-        <v>0.0103938610007936</v>
-      </c>
-      <c r="DQ2" s="6" t="n">
-        <v>0.010592811600659</v>
-      </c>
-      <c r="DR2" s="6" t="n">
-        <v>0.0107727388451816</v>
-      </c>
-      <c r="DS2" s="6" t="n">
-        <v>0.0109376717967745</v>
-      </c>
-      <c r="DT2" s="6" t="n">
-        <v>0.0110892342411869</v>
-      </c>
-      <c r="DU2" s="6" t="n">
-        <v>0.0112292836147036</v>
-      </c>
-      <c r="DV2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="DW2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="DX2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="DY2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="DZ2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="EA2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="EB2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="EC2" s="6" t="n">
-        <v>0.0113597737310146</v>
-      </c>
-      <c r="ED2" s="6" t="n">
-        <v>0.0113597737310146</v>
+        <v>94</v>
+      </c>
+      <c r="DJ2" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="DK2" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="DL2" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="DM2" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="DN2" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="DO2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="DP2" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="DQ2" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="DR2" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="DS2" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="DT2" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="DU2" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="DV2" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="DW2" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="DX2" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="DY2" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="DZ2" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="EA2" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="EB2" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="EC2" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="ED2" s="0" t="n">
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1629,350 +1624,350 @@
       <c r="S3" s="4" t="n">
         <v>0.00975964976190056</v>
       </c>
-      <c r="T3" s="4" t="n">
-        <v>0.00994369140614616</v>
-      </c>
-      <c r="U3" s="4" t="n">
-        <v>0.0100860993221696</v>
-      </c>
-      <c r="V3" s="4" t="n">
-        <v>0.0101962918529376</v>
-      </c>
-      <c r="W3" s="4" t="n">
-        <v>0.0102815567327007</v>
-      </c>
-      <c r="X3" s="4" t="n">
-        <v>0.0103475330712997</v>
-      </c>
-      <c r="Y3" s="4" t="n">
-        <v>0.0103985843044336</v>
-      </c>
-      <c r="Z3" s="4" t="n">
-        <v>0.0104380867754685</v>
-      </c>
-      <c r="AA3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AB3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AC3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AD3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AE3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AF3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AG3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AH3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AI3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AJ3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AK3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AL3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AM3" s="4" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="AN3" s="4" t="n">
-        <v>0.215660099459011</v>
-      </c>
-      <c r="AO3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="4" t="n">
-        <v>0.161742006487339</v>
-      </c>
-      <c r="AQ3" s="4" t="n">
-        <v>0.169308428599414</v>
-      </c>
-      <c r="AR3" s="4" t="n">
-        <v>0.176365904569944</v>
-      </c>
-      <c r="AS3" s="4" t="n">
-        <v>0.18297964163297</v>
-      </c>
-      <c r="AT3" s="4" t="n">
-        <v>0.189201221297133</v>
-      </c>
-      <c r="AU3" s="4" t="n">
-        <v>0.195072297087062</v>
-      </c>
-      <c r="AV3" s="4" t="n">
-        <v>0.20062713583778</v>
-      </c>
-      <c r="AW3" s="4" t="n">
-        <v>0.20589439882673</v>
-      </c>
-      <c r="AX3" s="4" t="n">
-        <v>0.210898413741575</v>
-      </c>
-      <c r="AY3" s="4" t="n">
-        <v>0.215660099459011</v>
-      </c>
-      <c r="AZ3" s="4" t="n">
-        <v>0.220197649997716</v>
-      </c>
-      <c r="BA3" s="4" t="n">
-        <v>0.224527048653529</v>
-      </c>
-      <c r="BB3" s="4" t="n">
-        <v>0.228662460479335</v>
-      </c>
-      <c r="BC3" s="4" t="n">
-        <v>0.232616536280382</v>
-      </c>
-      <c r="BD3" s="4" t="n">
-        <v>0.236400651311131</v>
-      </c>
-      <c r="BE3" s="4" t="n">
-        <v>0.240025095113871</v>
-      </c>
-      <c r="BF3" s="4" t="n">
-        <v>0.243499224317638</v>
-      </c>
-      <c r="BG3" s="4" t="n">
-        <v>0.246831587006463</v>
-      </c>
-      <c r="BH3" s="4" t="n">
-        <v>0.250030025007641</v>
-      </c>
-      <c r="BI3" s="4" t="n">
-        <v>0.253101758841433</v>
-      </c>
-      <c r="BJ3" s="4" t="n">
-        <v>0.256053458912728</v>
-      </c>
-      <c r="BK3" s="5" t="n">
-        <v>3.66466719485327</v>
-      </c>
-      <c r="BL3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM3" s="5" t="n">
-        <v>2.5717450599592</v>
-      </c>
-      <c r="BN3" s="5" t="n">
-        <v>2.70249467539181</v>
-      </c>
-      <c r="BO3" s="5" t="n">
-        <v>2.83020149854467</v>
-      </c>
-      <c r="BP3" s="5" t="n">
-        <v>2.95523022778606</v>
-      </c>
-      <c r="BQ3" s="5" t="n">
-        <v>3.07790237635853</v>
-      </c>
-      <c r="BR3" s="5" t="n">
-        <v>3.19850034358843</v>
-      </c>
-      <c r="BS3" s="5" t="n">
-        <v>3.31727174938514</v>
-      </c>
-      <c r="BT3" s="5" t="n">
-        <v>3.4344336442439</v>
-      </c>
-      <c r="BU3" s="5" t="n">
-        <v>3.55017639927116</v>
-      </c>
-      <c r="BV3" s="5" t="n">
-        <v>3.66466719485327</v>
-      </c>
-      <c r="BW3" s="5" t="n">
-        <v>3.77805309162941</v>
-      </c>
-      <c r="BX3" s="5" t="n">
-        <v>3.89046370225312</v>
-      </c>
-      <c r="BY3" s="5" t="n">
-        <v>4.00201349910886</v>
-      </c>
-      <c r="BZ3" s="5" t="n">
-        <v>4.1128037993041</v>
-      </c>
-      <c r="CA3" s="5" t="n">
-        <v>4.22292446858872</v>
-      </c>
-      <c r="CB3" s="5" t="n">
-        <v>4.3324553832003</v>
-      </c>
-      <c r="CC3" s="5" t="n">
-        <v>4.44146768465942</v>
-      </c>
-      <c r="CD3" s="5" t="n">
-        <v>4.55002485818068</v>
-      </c>
-      <c r="CE3" s="5" t="n">
-        <v>4.65818366112298</v>
-      </c>
-      <c r="CF3" s="5" t="n">
-        <v>4.76599492401657</v>
-      </c>
-      <c r="CG3" s="5" t="n">
-        <v>4.87350424326987</v>
-      </c>
-      <c r="CH3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="CI3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="CJ3" s="6" t="n">
-        <v>0.0105732047391501</v>
+      <c r="T3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AB3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="AE3" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="AF3" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AG3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="AH3" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="AI3" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="AJ3" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AK3" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="AL3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM3" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AN3" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="AO3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="AP3" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AQ3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AR3" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="AS3" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AT3" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AU3" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="AV3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW3" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="AX3" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AY3" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="AZ3" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="BA3" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="BB3" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="BC3" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="BD3" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="BE3" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="BF3" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="BG3" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="BH3" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="BI3" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="BJ3" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="BK3" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="BL3" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="BM3" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="BN3" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="BO3" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="BP3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="BQ3" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="BR3" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="BS3" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="BT3" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="BU3" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="BV3" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="BW3" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="BX3" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="BY3" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="BZ3" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="CA3" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="CB3" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="CC3" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="CD3" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="CE3" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="CF3" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="CG3" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="CH3" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="CI3" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="CJ3" s="0" t="n">
+        <v>70</v>
       </c>
       <c r="CK3" s="0" t="n">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="CL3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM3" s="6" t="n">
-        <v>0.00975964976190056</v>
-      </c>
-      <c r="CN3" s="6" t="n">
-        <v>0.00994369140614616</v>
-      </c>
-      <c r="CO3" s="6" t="n">
-        <v>0.0100860993221696</v>
-      </c>
-      <c r="CP3" s="6" t="n">
-        <v>0.0101962918529376</v>
-      </c>
-      <c r="CQ3" s="6" t="n">
-        <v>0.0102815567327007</v>
-      </c>
-      <c r="CR3" s="6" t="n">
-        <v>0.0103475330712997</v>
-      </c>
-      <c r="CS3" s="6" t="n">
-        <v>0.0103985843044336</v>
-      </c>
-      <c r="CT3" s="6" t="n">
-        <v>0.0104380867754685</v>
-      </c>
-      <c r="CU3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="CV3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="CW3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="CX3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="CY3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="CZ3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DA3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DB3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DC3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DD3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DE3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DF3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DG3" s="6" t="n">
-        <v>0.0105732047391501</v>
+        <v>72</v>
+      </c>
+      <c r="CM3" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="CN3" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="CO3" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="CP3" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="CQ3" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="CR3" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="CS3" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="CT3" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="CU3" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="CV3" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="CW3" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="CX3" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="CY3" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="CZ3" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="DA3" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="DB3" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="DC3" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="DD3" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="DE3" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="DF3" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="DG3" s="0" t="n">
+        <v>93</v>
       </c>
       <c r="DH3" s="0" t="n">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="DI3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="DJ3" s="6" t="n">
-        <v>0.00975964976190056</v>
-      </c>
-      <c r="DK3" s="6" t="n">
-        <v>0.00994369140614616</v>
-      </c>
-      <c r="DL3" s="6" t="n">
-        <v>0.0100860993221696</v>
-      </c>
-      <c r="DM3" s="6" t="n">
-        <v>0.0101962918529376</v>
-      </c>
-      <c r="DN3" s="6" t="n">
-        <v>0.0102815567327007</v>
-      </c>
-      <c r="DO3" s="6" t="n">
-        <v>0.0103475330712997</v>
-      </c>
-      <c r="DP3" s="6" t="n">
-        <v>0.0103985843044336</v>
-      </c>
-      <c r="DQ3" s="6" t="n">
-        <v>0.0104380867754685</v>
-      </c>
-      <c r="DR3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DS3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DT3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DU3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DV3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DW3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DX3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DY3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="DZ3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="EA3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="EB3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="EC3" s="6" t="n">
-        <v>0.0105732047391501</v>
-      </c>
-      <c r="ED3" s="6" t="n">
-        <v>0.0105732047391501</v>
+        <v>95</v>
+      </c>
+      <c r="DJ3" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="DK3" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="DL3" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="DM3" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="DN3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="DO3" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="DP3" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="DQ3" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="DR3" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="DS3" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="DT3" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="DU3" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="DV3" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="DW3" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="DX3" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="DY3" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="DZ3" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="EA3" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="EB3" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="EC3" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="ED3" s="0" t="n">
+        <v>116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,350 +2004,350 @@
       <c r="S4" s="4" t="n">
         <v>0.0107512900860089</v>
       </c>
-      <c r="T4" s="4" t="n">
-        <v>0.0109540314910248</v>
-      </c>
-      <c r="U4" s="4" t="n">
-        <v>0.011110908925468</v>
-      </c>
-      <c r="V4" s="4" t="n">
-        <v>0.0112322976937641</v>
-      </c>
-      <c r="W4" s="4" t="n">
-        <v>0.0113262260086982</v>
-      </c>
-      <c r="X4" s="4" t="n">
-        <v>0.0113989059482857</v>
-      </c>
-      <c r="Y4" s="4" t="n">
-        <v>0.0114551443000772</v>
-      </c>
-      <c r="Z4" s="4" t="n">
-        <v>0.0114986604646499</v>
-      </c>
-      <c r="AA4" s="4" t="n">
-        <v>0.0115323324432693</v>
-      </c>
-      <c r="AB4" s="4" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="AC4" s="4" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="AD4" s="4" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="AE4" s="4" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="AF4" s="4" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="AG4" s="4" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="AH4" s="4" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="AI4" s="4" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="AJ4" s="4" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="AK4" s="4" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="AL4" s="4" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="AM4" s="4" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="AN4" s="4" t="n">
-        <v>0.187527283268678</v>
-      </c>
-      <c r="AO4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="4" t="n">
-        <v>0.137420567841851</v>
-      </c>
-      <c r="AQ4" s="4" t="n">
-        <v>0.14518670026072</v>
-      </c>
-      <c r="AR4" s="4" t="n">
-        <v>0.152267364718126</v>
-      </c>
-      <c r="AS4" s="4" t="n">
-        <v>0.158730327559906</v>
-      </c>
-      <c r="AT4" s="4" t="n">
-        <v>0.164636264320935</v>
-      </c>
-      <c r="AU4" s="4" t="n">
-        <v>0.170039522509026</v>
-      </c>
-      <c r="AV4" s="4" t="n">
-        <v>0.174988801150333</v>
-      </c>
-      <c r="AW4" s="4" t="n">
-        <v>0.179527756253553</v>
-      </c>
-      <c r="AX4" s="4" t="n">
-        <v>0.183695540337784</v>
-      </c>
-      <c r="AY4" s="4" t="n">
-        <v>0.187527283268678</v>
-      </c>
-      <c r="AZ4" s="4" t="n">
-        <v>0.191054520847238</v>
-      </c>
-      <c r="BA4" s="4" t="n">
-        <v>0.194305576883955</v>
-      </c>
-      <c r="BB4" s="4" t="n">
-        <v>0.197305903858299</v>
-      </c>
-      <c r="BC4" s="4" t="n">
-        <v>0.200078386700897</v>
-      </c>
-      <c r="BD4" s="4" t="n">
-        <v>0.20264361373546</v>
-      </c>
-      <c r="BE4" s="4" t="n">
-        <v>0.205020118372582</v>
-      </c>
-      <c r="BF4" s="4" t="n">
-        <v>0.20722459475188</v>
-      </c>
-      <c r="BG4" s="4" t="n">
-        <v>0.209272090177042</v>
-      </c>
-      <c r="BH4" s="4" t="n">
-        <v>0.211176176875373</v>
-      </c>
-      <c r="BI4" s="4" t="n">
-        <v>0.212949105335091</v>
-      </c>
-      <c r="BJ4" s="4" t="n">
-        <v>0.214601941225974</v>
-      </c>
-      <c r="BK4" s="5" t="n">
-        <v>2.20461095678275</v>
-      </c>
-      <c r="BL4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM4" s="5" t="n">
-        <v>1.58340161570978</v>
-      </c>
-      <c r="BN4" s="5" t="n">
-        <v>1.64857486008002</v>
-      </c>
-      <c r="BO4" s="5" t="n">
-        <v>1.71481485521479</v>
-      </c>
-      <c r="BP4" s="5" t="n">
-        <v>1.78207616809426</v>
-      </c>
-      <c r="BQ4" s="5" t="n">
-        <v>1.85031366005566</v>
-      </c>
-      <c r="BR4" s="5" t="n">
-        <v>1.91948271150601</v>
-      </c>
-      <c r="BS4" s="5" t="n">
-        <v>1.98953942398276</v>
-      </c>
-      <c r="BT4" s="5" t="n">
-        <v>2.06044079912017</v>
-      </c>
-      <c r="BU4" s="5" t="n">
-        <v>2.13214489450518</v>
-      </c>
-      <c r="BV4" s="5" t="n">
-        <v>2.20461095678275</v>
-      </c>
-      <c r="BW4" s="5" t="n">
-        <v>2.27779953269489</v>
-      </c>
-      <c r="BX4" s="5" t="n">
-        <v>2.35167255900863</v>
-      </c>
-      <c r="BY4" s="5" t="n">
-        <v>2.42619343250563</v>
-      </c>
-      <c r="BZ4" s="5" t="n">
-        <v>2.50132706137321</v>
-      </c>
-      <c r="CA4" s="5" t="n">
-        <v>2.57703989945536</v>
-      </c>
-      <c r="CB4" s="5" t="n">
-        <v>2.653299964898</v>
-      </c>
-      <c r="CC4" s="5" t="n">
-        <v>2.73007684475868</v>
-      </c>
-      <c r="CD4" s="5" t="n">
-        <v>2.80734168715401</v>
-      </c>
-      <c r="CE4" s="5" t="n">
-        <v>2.88506718249131</v>
-      </c>
-      <c r="CF4" s="5" t="n">
-        <v>2.96322753528089</v>
-      </c>
-      <c r="CG4" s="5" t="n">
-        <v>3.04179842795671</v>
-      </c>
-      <c r="CH4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="CI4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="CJ4" s="6" t="n">
-        <v>0.011647507242845</v>
+      <c r="T4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="AC4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="AE4" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AF4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="AG4" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="AH4" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="AI4" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AJ4" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="AK4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="AL4" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AM4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="AN4" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO4" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AP4" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AQ4" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="AR4" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AS4" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AT4" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="AU4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AV4" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="AW4" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AX4" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="AY4" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="AZ4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="BA4" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="BB4" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="BC4" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="BD4" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="BE4" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="BF4" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="BG4" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="BH4" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="BI4" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="BJ4" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="BK4" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="BL4" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="BM4" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="BN4" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="BO4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="BP4" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="BQ4" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="BR4" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="BS4" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="BT4" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="BU4" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="BV4" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="BW4" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="BX4" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="BY4" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="BZ4" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="CA4" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="CB4" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="CC4" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="CD4" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="CE4" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="CF4" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="CG4" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="CH4" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="CI4" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="CJ4" s="0" t="n">
+        <v>71</v>
       </c>
       <c r="CK4" s="0" t="n">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="CL4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM4" s="6" t="n">
-        <v>0.0107512900860089</v>
-      </c>
-      <c r="CN4" s="6" t="n">
-        <v>0.0109540314910248</v>
-      </c>
-      <c r="CO4" s="6" t="n">
-        <v>0.011110908925468</v>
-      </c>
-      <c r="CP4" s="6" t="n">
-        <v>0.0112322976937641</v>
-      </c>
-      <c r="CQ4" s="6" t="n">
-        <v>0.0113262260086982</v>
-      </c>
-      <c r="CR4" s="6" t="n">
-        <v>0.0113989059482857</v>
-      </c>
-      <c r="CS4" s="6" t="n">
-        <v>0.0114551443000772</v>
-      </c>
-      <c r="CT4" s="6" t="n">
-        <v>0.0114986604646499</v>
-      </c>
-      <c r="CU4" s="6" t="n">
-        <v>0.0115323324432693</v>
-      </c>
-      <c r="CV4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="CW4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="CX4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="CY4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="CZ4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DA4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DB4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DC4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DD4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DE4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DF4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DG4" s="6" t="n">
-        <v>0.011647507242845</v>
+        <v>73</v>
+      </c>
+      <c r="CM4" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="CN4" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="CO4" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="CP4" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="CQ4" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="CR4" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="CS4" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="CT4" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="CU4" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="CV4" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="CW4" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="CX4" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="CY4" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="CZ4" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="DA4" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="DB4" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="DC4" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="DD4" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="DE4" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="DF4" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="DG4" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="DH4" s="0" t="n">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="DI4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="DJ4" s="6" t="n">
-        <v>0.0107512900860089</v>
-      </c>
-      <c r="DK4" s="6" t="n">
-        <v>0.0109540314910248</v>
-      </c>
-      <c r="DL4" s="6" t="n">
-        <v>0.011110908925468</v>
-      </c>
-      <c r="DM4" s="6" t="n">
-        <v>0.0112322976937641</v>
-      </c>
-      <c r="DN4" s="6" t="n">
-        <v>0.0113262260086982</v>
-      </c>
-      <c r="DO4" s="6" t="n">
-        <v>0.0113989059482857</v>
-      </c>
-      <c r="DP4" s="6" t="n">
-        <v>0.0114551443000772</v>
-      </c>
-      <c r="DQ4" s="6" t="n">
-        <v>0.0114986604646499</v>
-      </c>
-      <c r="DR4" s="6" t="n">
-        <v>0.0115323324432693</v>
-      </c>
-      <c r="DS4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DT4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DU4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DV4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DW4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DX4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DY4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="DZ4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="EA4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="EB4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="EC4" s="6" t="n">
-        <v>0.011647507242845</v>
-      </c>
-      <c r="ED4" s="6" t="n">
-        <v>0.011647507242845</v>
+        <v>96</v>
+      </c>
+      <c r="DJ4" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="DK4" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="DL4" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="DM4" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="DN4" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="DO4" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="DP4" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="DQ4" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="DR4" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="DS4" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="DT4" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="DU4" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="DV4" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="DW4" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="DX4" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="DY4" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="DZ4" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="EA4" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="EB4" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="EC4" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="ED4" s="0" t="n">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2374,7 +2369,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="M4 D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2388,15 +2383,15 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>137</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -2404,7 +2399,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>138</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -2412,7 +2407,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>139</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -2420,7 +2415,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>140</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -2428,7 +2423,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>141</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -2436,7 +2431,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -2444,7 +2439,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -2452,7 +2447,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -2460,7 +2455,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>145</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -2468,7 +2463,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -2476,7 +2471,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B12" s="0" t="n">
@@ -2484,7 +2479,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B13" s="0" t="n">
@@ -2492,7 +2487,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B14" s="0" t="n">
@@ -2500,7 +2495,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>150</v>
       </c>
       <c r="B15" s="0" t="n">
@@ -2508,7 +2503,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="6" t="s">
         <v>151</v>
       </c>
       <c r="B16" s="0" t="n">
@@ -2516,7 +2511,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>152</v>
       </c>
       <c r="B17" s="0" t="n">
@@ -2524,7 +2519,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
         <v>153</v>
       </c>
       <c r="B18" s="0" t="n">
@@ -2532,7 +2527,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="6" t="s">
         <v>154</v>
       </c>
       <c r="B19" s="0" t="n">
@@ -2540,7 +2535,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="6" t="s">
         <v>155</v>
       </c>
       <c r="B20" s="0" t="n">
@@ -2548,7 +2543,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="6" t="s">
         <v>156</v>
       </c>
       <c r="B21" s="0" t="n">
@@ -2556,7 +2551,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="6" t="s">
         <v>157</v>
       </c>
       <c r="B22" s="0" t="n">
@@ -2564,7 +2559,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="6" t="s">
         <v>158</v>
       </c>
       <c r="B23" s="0" t="n">
@@ -2590,7 +2585,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="M4 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2609,26 +2604,26 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="10" t="n">
+      <c r="B2" s="8" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="10" t="n">
+      <c r="B3" s="8" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="10" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -2651,7 +2646,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
+      <selection pane="topLeft" activeCell="M17" activeCellId="1" sqref="M4 M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2711,28 +2706,28 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="7" t="s">
         <v>132</v>
       </c>
       <c r="O2" s="0" t="n">
@@ -2743,28 +2738,28 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="7" t="s">
         <v>172</v>
       </c>
       <c r="O3" s="0" t="n">
@@ -2775,28 +2770,28 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="7" t="s">
         <v>132</v>
       </c>
       <c r="O4" s="0" t="n">
@@ -2807,28 +2802,28 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="7" t="s">
         <v>172</v>
       </c>
       <c r="O5" s="0" t="n">
@@ -2839,28 +2834,28 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="7" t="s">
         <v>132</v>
       </c>
       <c r="O6" s="0" t="n">
@@ -2871,28 +2866,28 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="N7" s="7" t="s">
         <v>172</v>
       </c>
       <c r="O7" s="0" t="n">
@@ -2921,7 +2916,7 @@
   <dimension ref="B11:Z16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="M4 B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2930,464 +2925,464 @@
   </cols>
   <sheetData>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="n">
+      <c r="B11" s="9" t="n">
         <v>0.517060418158145</v>
       </c>
-      <c r="C11" s="6" t="n">
+      <c r="C11" s="9" t="n">
         <v>0.00477309647620454</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="9" t="n">
         <v>0.0109376717967745</v>
       </c>
-      <c r="E11" s="6" t="n">
+      <c r="E11" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="6" t="n">
+      <c r="F11" s="9" t="n">
         <v>0.0085542471378061</v>
       </c>
-      <c r="G11" s="6" t="n">
+      <c r="G11" s="9" t="n">
         <v>0.0089680061019089</v>
       </c>
-      <c r="H11" s="6" t="n">
+      <c r="H11" s="9" t="n">
         <v>0.00932918878322026</v>
       </c>
-      <c r="I11" s="6" t="n">
+      <c r="I11" s="9" t="n">
         <v>0.0096459956148867</v>
       </c>
-      <c r="J11" s="6" t="n">
+      <c r="J11" s="9" t="n">
         <v>0.00992592896344995</v>
       </c>
-      <c r="K11" s="6" t="n">
+      <c r="K11" s="9" t="n">
         <v>0.0101729924814026</v>
       </c>
-      <c r="L11" s="6" t="n">
+      <c r="L11" s="9" t="n">
         <v>0.0103938610007936</v>
       </c>
-      <c r="M11" s="6" t="n">
+      <c r="M11" s="9" t="n">
         <v>0.010592811600659</v>
       </c>
-      <c r="N11" s="6" t="n">
+      <c r="N11" s="9" t="n">
         <v>0.0107727388451816</v>
       </c>
-      <c r="O11" s="6" t="n">
+      <c r="O11" s="9" t="n">
         <v>0.0109376717967745</v>
       </c>
-      <c r="P11" s="6" t="n">
+      <c r="P11" s="9" t="n">
         <v>0.0110892342411869</v>
       </c>
-      <c r="Q11" s="6" t="n">
+      <c r="Q11" s="9" t="n">
         <v>0.0112292836147036</v>
       </c>
-      <c r="R11" s="6" t="n">
+      <c r="R11" s="9" t="n">
         <v>0.0113597737310146</v>
       </c>
-      <c r="S11" s="6" t="n">
+      <c r="S11" s="9" t="n">
         <v>0.0113597737310146</v>
       </c>
-      <c r="T11" s="6" t="n">
+      <c r="T11" s="9" t="n">
         <v>0.0113597737310146</v>
       </c>
-      <c r="U11" s="6" t="n">
+      <c r="U11" s="9" t="n">
         <v>0.0113597737310146</v>
       </c>
-      <c r="V11" s="6" t="n">
+      <c r="V11" s="9" t="n">
         <v>0.0113597737310146</v>
       </c>
-      <c r="W11" s="6" t="n">
+      <c r="W11" s="9" t="n">
         <v>0.0113597737310146</v>
       </c>
-      <c r="X11" s="6" t="n">
+      <c r="X11" s="9" t="n">
         <v>0.0113597737310146</v>
       </c>
-      <c r="Y11" s="6" t="n">
+      <c r="Y11" s="9" t="n">
         <v>0.0113597737310146</v>
       </c>
-      <c r="Z11" s="6" t="n">
+      <c r="Z11" s="9" t="n">
         <v>0.0113597737310146</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="n">
+      <c r="B12" s="9" t="n">
         <v>0.681300623544814</v>
       </c>
-      <c r="C12" s="6" t="n">
+      <c r="C12" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="D12" s="6" t="n">
+      <c r="D12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="E12" s="6" t="n">
+      <c r="E12" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="6" t="n">
+      <c r="F12" s="9" t="n">
         <v>0.0378354562813396</v>
       </c>
-      <c r="G12" s="6" t="n">
+      <c r="G12" s="9" t="n">
         <v>0.038548934710861</v>
       </c>
-      <c r="H12" s="6" t="n">
+      <c r="H12" s="9" t="n">
         <v>0.0391010107189422</v>
       </c>
-      <c r="I12" s="6" t="n">
+      <c r="I12" s="9" t="n">
         <v>0.0395281966100464</v>
       </c>
-      <c r="J12" s="6" t="n">
+      <c r="J12" s="9" t="n">
         <v>0.0398587449093519</v>
       </c>
-      <c r="K12" s="6" t="n">
+      <c r="K12" s="9" t="n">
         <v>0.0401145168822775</v>
       </c>
-      <c r="L12" s="6" t="n">
+      <c r="L12" s="9" t="n">
         <v>0.0403124283592741</v>
       </c>
-      <c r="M12" s="6" t="n">
+      <c r="M12" s="9" t="n">
         <v>0.0404655684874865</v>
       </c>
-      <c r="N12" s="6" t="n">
+      <c r="N12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="O12" s="6" t="n">
+      <c r="O12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="P12" s="6" t="n">
+      <c r="P12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="Q12" s="6" t="n">
+      <c r="Q12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="R12" s="6" t="n">
+      <c r="R12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="S12" s="6" t="n">
+      <c r="S12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="T12" s="6" t="n">
+      <c r="T12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="U12" s="6" t="n">
+      <c r="U12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="V12" s="6" t="n">
+      <c r="V12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="W12" s="6" t="n">
+      <c r="W12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="X12" s="6" t="n">
+      <c r="X12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="Y12" s="6" t="n">
+      <c r="Y12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
-      <c r="Z12" s="6" t="n">
+      <c r="Z12" s="9" t="n">
         <v>0.0409893833714646</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6" t="n">
+      <c r="B13" s="9" t="n">
         <v>0.478489300184784</v>
       </c>
-      <c r="C13" s="6" t="n">
+      <c r="C13" s="9" t="n">
         <v>0.0233222234479954</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="E13" s="6" t="n">
+      <c r="E13" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="6" t="n">
+      <c r="F13" s="9" t="n">
         <v>0.00975964976190056</v>
       </c>
-      <c r="G13" s="6" t="n">
+      <c r="G13" s="9" t="n">
         <v>0.00994369140614616</v>
       </c>
-      <c r="H13" s="6" t="n">
+      <c r="H13" s="9" t="n">
         <v>0.0100860993221696</v>
       </c>
-      <c r="I13" s="6" t="n">
+      <c r="I13" s="9" t="n">
         <v>0.0101962918529376</v>
       </c>
-      <c r="J13" s="6" t="n">
+      <c r="J13" s="9" t="n">
         <v>0.0102815567327007</v>
       </c>
-      <c r="K13" s="6" t="n">
+      <c r="K13" s="9" t="n">
         <v>0.0103475330712997</v>
       </c>
-      <c r="L13" s="6" t="n">
+      <c r="L13" s="9" t="n">
         <v>0.0103985843044336</v>
       </c>
-      <c r="M13" s="6" t="n">
+      <c r="M13" s="9" t="n">
         <v>0.0104380867754685</v>
       </c>
-      <c r="N13" s="6" t="n">
+      <c r="N13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="O13" s="6" t="n">
+      <c r="O13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="P13" s="6" t="n">
+      <c r="P13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="Q13" s="6" t="n">
+      <c r="Q13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="R13" s="6" t="n">
+      <c r="R13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="S13" s="6" t="n">
+      <c r="S13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="T13" s="6" t="n">
+      <c r="T13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="U13" s="6" t="n">
+      <c r="U13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="V13" s="6" t="n">
+      <c r="V13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="W13" s="6" t="n">
+      <c r="W13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="X13" s="6" t="n">
+      <c r="X13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="Y13" s="6" t="n">
+      <c r="Y13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="Z13" s="6" t="n">
+      <c r="Z13" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6" t="n">
+      <c r="B14" s="9" t="n">
         <v>0.487368941136969</v>
       </c>
-      <c r="C14" s="6" t="n">
+      <c r="C14" s="9" t="n">
         <v>0.0281783726704106</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="E14" s="6" t="n">
+      <c r="E14" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="6" t="n">
+      <c r="F14" s="9" t="n">
         <v>0.0169722216830996</v>
       </c>
-      <c r="G14" s="6" t="n">
+      <c r="G14" s="9" t="n">
         <v>0.0172922736994385</v>
       </c>
-      <c r="H14" s="6" t="n">
+      <c r="H14" s="9" t="n">
         <v>0.0175399238486901</v>
       </c>
-      <c r="I14" s="6" t="n">
+      <c r="I14" s="9" t="n">
         <v>0.0177315508133499</v>
       </c>
-      <c r="J14" s="6" t="n">
+      <c r="J14" s="9" t="n">
         <v>0.0178798281057147</v>
       </c>
-      <c r="K14" s="6" t="n">
+      <c r="K14" s="9" t="n">
         <v>0.0179945622480107</v>
       </c>
-      <c r="L14" s="6" t="n">
+      <c r="L14" s="9" t="n">
         <v>0.0180833413401998</v>
       </c>
-      <c r="M14" s="6" t="n">
+      <c r="M14" s="9" t="n">
         <v>0.0181520369093842</v>
       </c>
-      <c r="N14" s="6" t="n">
+      <c r="N14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="O14" s="6" t="n">
+      <c r="O14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="P14" s="6" t="n">
+      <c r="P14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="Q14" s="6" t="n">
+      <c r="Q14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="R14" s="6" t="n">
+      <c r="R14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="S14" s="6" t="n">
+      <c r="S14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="T14" s="6" t="n">
+      <c r="T14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="U14" s="6" t="n">
+      <c r="U14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="V14" s="6" t="n">
+      <c r="V14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="W14" s="6" t="n">
+      <c r="W14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="X14" s="6" t="n">
+      <c r="X14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="Y14" s="6" t="n">
+      <c r="Y14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
-      <c r="Z14" s="6" t="n">
+      <c r="Z14" s="9" t="n">
         <v>0.0183870096890351</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="6" t="n">
+      <c r="B15" s="9" t="n">
         <v>0.480534834001414</v>
       </c>
-      <c r="C15" s="6" t="n">
+      <c r="C15" s="9" t="n">
         <v>0.0230853415702337</v>
       </c>
-      <c r="D15" s="6" t="n">
+      <c r="D15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
-      <c r="E15" s="6" t="n">
+      <c r="E15" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="6" t="n">
+      <c r="F15" s="9" t="n">
         <v>0.0107512900860089</v>
       </c>
-      <c r="G15" s="6" t="n">
+      <c r="G15" s="9" t="n">
         <v>0.0109540314910248</v>
       </c>
-      <c r="H15" s="6" t="n">
+      <c r="H15" s="9" t="n">
         <v>0.011110908925468</v>
       </c>
-      <c r="I15" s="6" t="n">
+      <c r="I15" s="9" t="n">
         <v>0.0112322976937641</v>
       </c>
-      <c r="J15" s="6" t="n">
+      <c r="J15" s="9" t="n">
         <v>0.0113262260086982</v>
       </c>
-      <c r="K15" s="6" t="n">
+      <c r="K15" s="9" t="n">
         <v>0.0113989059482857</v>
       </c>
-      <c r="L15" s="6" t="n">
+      <c r="L15" s="9" t="n">
         <v>0.0114551443000772</v>
       </c>
-      <c r="M15" s="6" t="n">
+      <c r="M15" s="9" t="n">
         <v>0.0114986604646499</v>
       </c>
-      <c r="N15" s="6" t="n">
+      <c r="N15" s="9" t="n">
         <v>0.0115323324432693</v>
       </c>
-      <c r="O15" s="6" t="n">
+      <c r="O15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
-      <c r="P15" s="6" t="n">
+      <c r="P15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
-      <c r="Q15" s="6" t="n">
+      <c r="Q15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
-      <c r="R15" s="6" t="n">
+      <c r="R15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
-      <c r="S15" s="6" t="n">
+      <c r="S15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
-      <c r="T15" s="6" t="n">
+      <c r="T15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
-      <c r="U15" s="6" t="n">
+      <c r="U15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
-      <c r="V15" s="6" t="n">
+      <c r="V15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
-      <c r="W15" s="6" t="n">
+      <c r="W15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
-      <c r="X15" s="6" t="n">
+      <c r="X15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
-      <c r="Y15" s="6" t="n">
+      <c r="Y15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
-      <c r="Z15" s="6" t="n">
+      <c r="Z15" s="9" t="n">
         <v>0.011647507242845</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="6" t="n">
+      <c r="B16" s="9" t="n">
         <v>0.478489300184784</v>
       </c>
-      <c r="C16" s="6" t="n">
+      <c r="C16" s="9" t="n">
         <v>0.0233222234479954</v>
       </c>
-      <c r="D16" s="6" t="n">
+      <c r="D16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="E16" s="6" t="n">
+      <c r="E16" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F16" s="6" t="n">
+      <c r="F16" s="9" t="n">
         <v>0.00975964976190056</v>
       </c>
-      <c r="G16" s="6" t="n">
+      <c r="G16" s="9" t="n">
         <v>0.00994369140614616</v>
       </c>
-      <c r="H16" s="6" t="n">
+      <c r="H16" s="9" t="n">
         <v>0.0100860993221696</v>
       </c>
-      <c r="I16" s="6" t="n">
+      <c r="I16" s="9" t="n">
         <v>0.0101962918529376</v>
       </c>
-      <c r="J16" s="6" t="n">
+      <c r="J16" s="9" t="n">
         <v>0.0102815567327007</v>
       </c>
-      <c r="K16" s="6" t="n">
+      <c r="K16" s="9" t="n">
         <v>0.0103475330712997</v>
       </c>
-      <c r="L16" s="6" t="n">
+      <c r="L16" s="9" t="n">
         <v>0.0103985843044336</v>
       </c>
-      <c r="M16" s="6" t="n">
+      <c r="M16" s="9" t="n">
         <v>0.0104380867754685</v>
       </c>
-      <c r="N16" s="6" t="n">
+      <c r="N16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="O16" s="6" t="n">
+      <c r="O16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="P16" s="6" t="n">
+      <c r="P16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="Q16" s="6" t="n">
+      <c r="Q16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="R16" s="6" t="n">
+      <c r="R16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="S16" s="6" t="n">
+      <c r="S16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="T16" s="6" t="n">
+      <c r="T16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="U16" s="6" t="n">
+      <c r="U16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="V16" s="6" t="n">
+      <c r="V16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="W16" s="6" t="n">
+      <c r="W16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="X16" s="6" t="n">
+      <c r="X16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="Y16" s="6" t="n">
+      <c r="Y16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
-      <c r="Z16" s="6" t="n">
+      <c r="Z16" s="9" t="n">
         <v>0.0105732047391501</v>
       </c>
     </row>

</xml_diff>